<commit_message>
integrated the methods that parse the excel files with the current service
</commit_message>
<xml_diff>
--- a/src/main/resources/data/variables/Niguarda_v1.xlsx
+++ b/src/main/resources/data/variables/Niguarda_v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics.csv" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="92">
   <si>
     <t xml:space="preserve">csvFile</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t xml:space="preserve">conceptPath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">methodology</t>
   </si>
   <si>
     <t xml:space="preserve">Demographics</t>
@@ -335,8 +338,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="11"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -422,7 +424,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -432,6 +434,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,17 +486,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -524,56 +530,59 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="H2" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
+      <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="H3" s="8" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8" t="s">
         <v>21</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -592,19 +601,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="86.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.5867346938775"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -638,302 +647,305 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="H2" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
+      <c r="A3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="7" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="G3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="A4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="A5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="H5" s="8" t="s">
         <v>31</v>
       </c>
+      <c r="I5" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="7" t="s">
+      <c r="A6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="7" t="s">
+      <c r="A7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>35</v>
       </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="7" t="s">
+      <c r="A8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>37</v>
       </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="7" t="s">
+      <c r="A9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>39</v>
       </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="7" t="s">
+      <c r="A10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>41</v>
       </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="7" t="s">
+      <c r="A11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>43</v>
       </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="7" t="s">
+      <c r="A12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>45</v>
       </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="7" t="s">
+      <c r="A13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>47</v>
       </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="7" t="s">
+      <c r="A14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>49</v>
       </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="7" t="s">
+      <c r="A15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>51</v>
       </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="7" t="s">
+      <c r="A16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>53</v>
       </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="7" t="s">
+      <c r="A17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>55</v>
       </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="7" t="s">
+      <c r="A18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="7" t="s">
+      <c r="A19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>59</v>
       </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="7" t="s">
+      <c r="A20" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>61</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -952,19 +964,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="76.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -998,242 +1010,245 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="A2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="H2" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
+      <c r="A3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="7" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="G3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="A4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>64</v>
       </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="7" t="s">
+      <c r="A5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>66</v>
       </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="A6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="H6" s="10" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="7" t="s">
+      <c r="A7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>71</v>
       </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="7" t="s">
+      <c r="A8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>73</v>
       </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="7" t="s">
+      <c r="A9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>75</v>
       </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="7" t="s">
+      <c r="A10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>77</v>
       </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="7" t="s">
+      <c r="A11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>79</v>
       </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="7" t="s">
+      <c r="A12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>81</v>
       </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="7" t="s">
+      <c r="A13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>83</v>
       </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" s="7" t="s">
+      <c r="A14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>85</v>
       </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" s="7" t="s">
+      <c r="A15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>87</v>
       </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="A16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>90</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>